<commit_message>
Update for 11-month environment
</commit_message>
<xml_diff>
--- a/L2CPE/L2CPE_raw.xlsx
+++ b/L2CPE/L2CPE_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adestefa\Documents\GitHub\SolarCruiserDose\L2CPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CF1E5B-6F8F-4706-A5BA-ECEC6051DC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCD50B9-E1D2-422D-AA70-A3894D58D953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DA6DCCD3-9449-49F8-BBEB-44C3E2ADBD74}"/>
   </bookViews>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8848DE37-3270-448E-9B5C-45DFB837CD05}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +418,7 @@
     <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <f>SQRT(B2*C2)</f>
         <v>1.3416407864998738E-3</v>
@@ -503,8 +503,24 @@
         <f>B2</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R2" s="2">
+        <f>A2</f>
+        <v>1.3416407864998738E-3</v>
+      </c>
+      <c r="S2" s="2">
+        <f>E2*(11/12)*365*24*3600*(1/(0.984)^2)</f>
+        <v>2353528033.9083877</v>
+      </c>
+      <c r="T2" s="2">
+        <f>C2-B2</f>
+        <v>7.9999999999999993E-4</v>
+      </c>
+      <c r="U2" s="2">
+        <f>B2</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A29" si="0">SQRT(B3*C3)</f>
         <v>2.3999999999999998E-3</v>
@@ -554,8 +570,24 @@
         <f t="shared" ref="P3:P29" si="3">B3</f>
         <v>1.8E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R3" s="2">
+        <f t="shared" ref="R3:R29" si="4">A3</f>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="S3" s="2">
+        <f t="shared" ref="S3:S29" si="5">E3*(11/12)*365*24*3600*(1/(0.984)^2)</f>
+        <v>3958871207.6145144</v>
+      </c>
+      <c r="T3" s="2">
+        <f t="shared" ref="T3:T29" si="6">C3-B3</f>
+        <v>1.4000000000000002E-3</v>
+      </c>
+      <c r="U3" s="2">
+        <f t="shared" ref="U3:U29" si="7">B3</f>
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>4.2332020977033447E-3</v>
@@ -605,8 +637,24 @@
         <f t="shared" si="3"/>
         <v>3.2000000000000002E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R4" s="2">
+        <f t="shared" si="4"/>
+        <v>4.2332020977033447E-3</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" si="5"/>
+        <v>6541392772.1594296</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="6"/>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="7"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>7.4833147735478825E-3</v>
@@ -656,8 +704,24 @@
         <f t="shared" si="3"/>
         <v>5.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R5" s="2">
+        <f t="shared" si="4"/>
+        <v>7.4833147735478825E-3</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" si="5"/>
+        <v>10580874479.476501</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="6"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" si="7"/>
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>1.3341664064126334E-2</v>
@@ -707,8 +771,24 @@
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R6" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3341664064126334E-2</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="5"/>
+        <v>16575907198.096373</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="6"/>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="7"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2.3716660810493541E-2</v>
@@ -758,8 +838,24 @@
         <f t="shared" si="3"/>
         <v>1.78E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R7" s="2">
+        <f t="shared" si="4"/>
+        <v>2.3716660810493541E-2</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="5"/>
+        <v>25057923111.243305</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3800000000000003E-2</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="7"/>
+        <v>1.78E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>4.2141665842726252E-2</v>
@@ -809,8 +905,24 @@
         <f t="shared" si="3"/>
         <v>3.1600000000000003E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R8" s="2">
+        <f t="shared" si="4"/>
+        <v>4.2141665842726252E-2</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="5"/>
+        <v>36274724866.1511</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="6"/>
+        <v>2.4599999999999997E-2</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="7"/>
+        <v>3.1600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>7.4966659255965254E-2</v>
@@ -860,8 +972,24 @@
         <f t="shared" si="3"/>
         <v>5.62E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R9" s="2">
+        <f t="shared" si="4"/>
+        <v>7.4966659255965254E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="5"/>
+        <v>49739663890.541336</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="6"/>
+        <v>4.3800000000000006E-2</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="7"/>
+        <v>5.62E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>0.13334166640626627</v>
@@ -911,8 +1039,24 @@
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.13334166640626627</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="5"/>
+        <v>64757101427.721596</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="6"/>
+        <v>7.7800000000000008E-2</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="7"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>0.23710832967232509</v>
@@ -962,8 +1106,24 @@
         <f t="shared" si="3"/>
         <v>0.17780000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.23710832967232509</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="5"/>
+        <v>77774204342.653183</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="6"/>
+        <v>0.13839999999999997</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="7"/>
+        <v>0.17780000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>0.42166249536803718</v>
@@ -1013,8 +1173,24 @@
         <f t="shared" si="3"/>
         <v>0.31619999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.42166249536803718</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="5"/>
+        <v>88134146341.463425</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="6"/>
+        <v>0.24610000000000004</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="7"/>
+        <v>0.31619999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>0.74986665481270731</v>
@@ -1064,8 +1240,24 @@
         <f t="shared" si="3"/>
         <v>0.56230000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.74986665481270731</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="5"/>
+        <v>91686979476.502075</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="6"/>
+        <v>0.43769999999999998</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="7"/>
+        <v>0.56230000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>1.3335291522872681</v>
@@ -1115,8 +1307,24 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R14" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3335291522872681</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="5"/>
+        <v>88850684116.597275</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="6"/>
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2.371395810487992</v>
@@ -1166,8 +1374,24 @@
         <f t="shared" si="3"/>
         <v>1.7783</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R15" s="2">
+        <f t="shared" si="4"/>
+        <v>2.371395810487992</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="5"/>
+        <v>79684971743.010101</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3840000000000001</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="7"/>
+        <v>1.7783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>4.2169749607983205</v>
@@ -1217,8 +1441,24 @@
         <f t="shared" si="3"/>
         <v>3.1623000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R16" s="2">
+        <f t="shared" si="4"/>
+        <v>4.2169749607983205</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="5"/>
+        <v>66339455681.142181</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="6"/>
+        <v>2.4611000000000001</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="7"/>
+        <v>3.1623000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>7.4989332574706919</v>
@@ -1268,8 +1508,24 @@
         <f t="shared" si="3"/>
         <v>5.6234000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R17" s="2">
+        <f t="shared" si="4"/>
+        <v>7.4989332574706919</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="5"/>
+        <v>51978844437.834618</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="6"/>
+        <v>4.3765999999999998</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="7"/>
+        <v>5.6234000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>13.335216533675036</v>
@@ -1319,8 +1575,24 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R18" s="2">
+        <f t="shared" si="4"/>
+        <v>13.335216533675036</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="5"/>
+        <v>38872174301.011307</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="6"/>
+        <v>7.7828000000000017</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>23.713749763375677</v>
@@ -1370,8 +1642,24 @@
         <f t="shared" si="3"/>
         <v>17.782800000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R19" s="2">
+        <f t="shared" si="4"/>
+        <v>23.713749763375677</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="5"/>
+        <v>27198579714.455677</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="6"/>
+        <v>13.84</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" si="7"/>
+        <v>17.782800000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>42.16965375100915</v>
@@ -1421,8 +1709,24 @@
         <f t="shared" si="3"/>
         <v>31.622800000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R20" s="2">
+        <f t="shared" si="4"/>
+        <v>42.16965375100915</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="5"/>
+        <v>18486674598.453304</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="6"/>
+        <v>24.611299999999996</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" si="7"/>
+        <v>31.622800000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>74.989399250827447</v>
@@ -1472,8 +1776,24 @@
         <f t="shared" si="3"/>
         <v>56.234099999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R21" s="2">
+        <f t="shared" si="4"/>
+        <v>74.989399250827447</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="5"/>
+        <v>12109488399.762047</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="6"/>
+        <v>43.765900000000002</v>
+      </c>
+      <c r="U21" s="2">
+        <f t="shared" si="7"/>
+        <v>56.234099999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>133.35212784204083</v>
@@ -1523,8 +1843,24 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R22" s="2">
+        <f t="shared" si="4"/>
+        <v>133.35212784204083</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="5"/>
+        <v>7810261748.9589539</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="6"/>
+        <v>77.8279</v>
+      </c>
+      <c r="U22" s="2">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>237.13735596826578</v>
@@ -1574,8 +1910,24 @@
         <f t="shared" si="3"/>
         <v>177.8279</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R23" s="2">
+        <f t="shared" si="4"/>
+        <v>237.13735596826578</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="5"/>
+        <v>4923211629.9821539</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="6"/>
+        <v>138.3999</v>
+      </c>
+      <c r="U23" s="2">
+        <f t="shared" si="7"/>
+        <v>177.8279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>421.69651664217008</v>
@@ -1625,8 +1977,24 @@
         <f t="shared" si="3"/>
         <v>316.2278</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R24" s="2">
+        <f t="shared" si="4"/>
+        <v>421.69651664217008</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="5"/>
+        <v>3042299970.2558002</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="6"/>
+        <v>246.11350000000004</v>
+      </c>
+      <c r="U24" s="2">
+        <f t="shared" si="7"/>
+        <v>316.2278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>749.89419253652045</v>
@@ -1676,8 +2044,24 @@
         <f t="shared" si="3"/>
         <v>562.34130000000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R25" s="2">
+        <f t="shared" si="4"/>
+        <v>749.89419253652045</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="5"/>
+        <v>1850160246.8768592</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="6"/>
+        <v>437.65869999999995</v>
+      </c>
+      <c r="U25" s="2">
+        <f t="shared" si="7"/>
+        <v>562.34130000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>1333.5214283992589</v>
@@ -1727,8 +2111,24 @@
         <f t="shared" si="3"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R26" s="2">
+        <f t="shared" si="4"/>
+        <v>1333.5214283992589</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="5"/>
+        <v>1114216240.3331351</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="6"/>
+        <v>778.2793999999999</v>
+      </c>
+      <c r="U26" s="2">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2371.3736764081359</v>
@@ -1778,8 +2178,24 @@
         <f t="shared" si="3"/>
         <v>1778.2793999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R27" s="2">
+        <f t="shared" si="4"/>
+        <v>2371.3736764081359</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="5"/>
+        <v>675038295.65734684</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="6"/>
+        <v>1383.9982</v>
+      </c>
+      <c r="U27" s="2">
+        <f t="shared" si="7"/>
+        <v>1778.2793999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>4216.9649372121366</v>
@@ -1829,8 +2245,24 @@
         <f t="shared" si="3"/>
         <v>3162.2775999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R28" s="2">
+        <f t="shared" si="4"/>
+        <v>4216.9649372121366</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="5"/>
+        <v>402156826.29387265</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="6"/>
+        <v>2461.1354999999999</v>
+      </c>
+      <c r="U28" s="2">
+        <f t="shared" si="7"/>
+        <v>3162.2775999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>7498.9419920412774</v>
@@ -1878,6 +2310,22 @@
       </c>
       <c r="P29" s="2">
         <f t="shared" si="3"/>
+        <v>5623.4130999999998</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="4"/>
+        <v>7498.9419920412774</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="5"/>
+        <v>238845925.04461631</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" si="6"/>
+        <v>4376.5869000000002</v>
+      </c>
+      <c r="U29" s="2">
+        <f t="shared" si="7"/>
         <v>5623.4130999999998</v>
       </c>
     </row>

</xml_diff>